<commit_message>
correcion de oanda sobre NaN
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -453,7 +453,7 @@
         <v>USD CRC</v>
       </c>
       <c r="C3">
-        <v>576.23</v>
+        <v>586.26</v>
       </c>
       <c r="D3" t="str">
         <v/>
@@ -465,7 +465,7 @@
         <v>EUR USD</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>1.07305</v>
       </c>
     </row>
     <row r="4">
@@ -476,7 +476,7 @@
         <v>USD UYU</v>
       </c>
       <c r="C4">
-        <v>39.119</v>
+        <v>39.092</v>
       </c>
       <c r="D4" t="str">
         <v/>
@@ -488,7 +488,7 @@
         <v>EUR COP</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>5091.85</v>
       </c>
     </row>
     <row r="5">
@@ -499,7 +499,7 @@
         <v>USD COP</v>
       </c>
       <c r="C5">
-        <v>4669.74</v>
+        <v>4775.99</v>
       </c>
       <c r="D5" t="str">
         <v/>
@@ -511,7 +511,7 @@
         <v>CNY USD</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.14734</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         <v>USD PEN</v>
       </c>
       <c r="C6">
-        <v>3.847</v>
+        <v>3.856</v>
       </c>
       <c r="D6" t="str">
         <v/>
@@ -534,7 +534,7 @@
         <v>JPY USD</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.00762</v>
       </c>
     </row>
     <row r="7">
@@ -545,7 +545,7 @@
         <v>EUR PEN</v>
       </c>
       <c r="C7">
-        <v>4.319</v>
+        <v>4.208</v>
       </c>
       <c r="D7" t="str">
         <v/>
@@ -557,7 +557,7 @@
         <v>CNY COP</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>699.156</v>
       </c>
     </row>
     <row r="8">
@@ -568,7 +568,7 @@
         <v>USD CLP</v>
       </c>
       <c r="C8">
-        <v>788.88</v>
+        <v>799.46</v>
       </c>
       <c r="D8" t="str">
         <v/>
@@ -580,7 +580,7 @@
         <v>JPY COP</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>36.1777</v>
       </c>
     </row>
     <row r="9">
@@ -591,7 +591,7 @@
         <v>EUR CLP</v>
       </c>
       <c r="C9">
-        <v>854.23</v>
+        <v>855.22</v>
       </c>
       <c r="D9" t="str">
         <v/>
@@ -603,7 +603,7 @@
         <v>BRL USD</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.192</v>
       </c>
     </row>
     <row r="10">
@@ -623,7 +623,7 @@
         <v>KRW USD</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>0.00079</v>
       </c>
     </row>
     <row r="11">
@@ -633,9 +633,6 @@
       <c r="B11" t="str">
         <v>USD HNL</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
       <c r="D11" t="str">
         <v/>
       </c>
@@ -646,7 +643,7 @@
         <v>USD CLP</v>
       </c>
       <c r="G11">
-        <v>NaN</v>
+        <v>797.331</v>
       </c>
     </row>
     <row r="12">
@@ -669,7 +666,7 @@
         <v>EUR CLP</v>
       </c>
       <c r="G12">
-        <v>860.728</v>
+        <v>855.699</v>
       </c>
     </row>
     <row r="13">
@@ -691,9 +688,6 @@
       <c r="F13" t="str">
         <v>BRL HNL</v>
       </c>
-      <c r="G13">
-        <v>4.71569</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -714,9 +708,6 @@
       <c r="F14" t="str">
         <v>CNY HNL</v>
       </c>
-      <c r="G14">
-        <v>3.58708</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -737,9 +728,6 @@
       <c r="F15" t="str">
         <v>EUR HNL</v>
       </c>
-      <c r="G15">
-        <v>26.2319</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -760,9 +748,6 @@
       <c r="F16" t="str">
         <v>GBP HNL</v>
       </c>
-      <c r="G16">
-        <v>29.2872</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -783,9 +768,6 @@
       <c r="F17" t="str">
         <v>JPY HNL</v>
       </c>
-      <c r="G17">
-        <v>0.18515</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -806,9 +788,6 @@
       <c r="F18" t="str">
         <v>MXN HNL</v>
       </c>
-      <c r="G18">
-        <v>1.28102</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -829,9 +808,6 @@
       <c r="F19" t="str">
         <v>HKD USD</v>
       </c>
-      <c r="G19">
-        <v>0.12743</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -851,9 +827,6 @@
       </c>
       <c r="F20" t="str">
         <v>HKD HNL</v>
-      </c>
-      <c r="G20">
-        <v>3.09728</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcion Nan para Oanda 2.0
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -465,7 +465,7 @@
         <v>EUR USD</v>
       </c>
       <c r="G3">
-        <v>1.06167</v>
+        <v>1.0637</v>
       </c>
     </row>
     <row r="4">
@@ -488,7 +488,7 @@
         <v>EUR COP</v>
       </c>
       <c r="G4">
-        <v>5022.42</v>
+        <v>5010.88</v>
       </c>
     </row>
     <row r="5">
@@ -511,7 +511,7 @@
         <v>CNY USD</v>
       </c>
       <c r="G5">
-        <v>0.14407</v>
+        <v>0.14477</v>
       </c>
     </row>
     <row r="6">
@@ -534,7 +534,7 @@
         <v>JPY USD</v>
       </c>
       <c r="G6">
-        <v>0.00736</v>
+        <v>0.0074</v>
       </c>
     </row>
     <row r="7">
@@ -557,7 +557,7 @@
         <v>CNY COP</v>
       </c>
       <c r="G7">
-        <v>NaN</v>
+        <v>682.004</v>
       </c>
     </row>
     <row r="8">
@@ -580,7 +580,7 @@
         <v>JPY COP</v>
       </c>
       <c r="G8">
-        <v>34.8184</v>
+        <v>34.8572</v>
       </c>
     </row>
     <row r="9">
@@ -603,7 +603,7 @@
         <v>BRL USD</v>
       </c>
       <c r="G9">
-        <v>0.19293</v>
+        <v>0.19163</v>
       </c>
     </row>
     <row r="10">
@@ -643,7 +643,7 @@
         <v>USD CLP</v>
       </c>
       <c r="G11">
-        <v>797.349</v>
+        <v>798.585</v>
       </c>
     </row>
     <row r="12">
@@ -666,7 +666,7 @@
         <v>EUR CLP</v>
       </c>
       <c r="G12">
-        <v>846.649</v>
+        <v>849.71</v>
       </c>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
Correcion de tasas cuando no carga la pagina/ correcion de codigo
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -465,7 +465,7 @@
         <v>EUR USD</v>
       </c>
       <c r="G3">
-        <v>1.0637</v>
+        <v>1.06432</v>
       </c>
     </row>
     <row r="4">
@@ -488,7 +488,7 @@
         <v>EUR COP</v>
       </c>
       <c r="G4">
-        <v>5010.88</v>
+        <v>5013.8</v>
       </c>
     </row>
     <row r="5">
@@ -557,7 +557,7 @@
         <v>CNY COP</v>
       </c>
       <c r="G7">
-        <v>682.004</v>
+        <v>681.996</v>
       </c>
     </row>
     <row r="8">
@@ -568,7 +568,7 @@
         <v>USD CLP</v>
       </c>
       <c r="C8">
-        <v>NaN</v>
+        <v>797.19</v>
       </c>
       <c r="D8" t="str">
         <v/>
@@ -580,7 +580,7 @@
         <v>JPY COP</v>
       </c>
       <c r="G8">
-        <v>34.8572</v>
+        <v>34.8824</v>
       </c>
     </row>
     <row r="9">
@@ -591,7 +591,7 @@
         <v>EUR CLP</v>
       </c>
       <c r="C9">
-        <v>NaN</v>
+        <v>850.06</v>
       </c>
       <c r="D9" t="str">
         <v/>
@@ -633,6 +633,9 @@
       <c r="B11" t="str">
         <v>USD HNL</v>
       </c>
+      <c r="C11">
+        <v>NaN</v>
+      </c>
       <c r="D11" t="str">
         <v/>
       </c>
@@ -643,7 +646,7 @@
         <v>USD CLP</v>
       </c>
       <c r="G11">
-        <v>798.585</v>
+        <v>798.554</v>
       </c>
     </row>
     <row r="12">
@@ -666,7 +669,7 @@
         <v>EUR CLP</v>
       </c>
       <c r="G12">
-        <v>849.71</v>
+        <v>850.19</v>
       </c>
     </row>
     <row r="13">
@@ -688,6 +691,9 @@
       <c r="F13" t="str">
         <v>BRL HNL</v>
       </c>
+      <c r="G13">
+        <v>4.62898</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -708,6 +714,9 @@
       <c r="F14" t="str">
         <v>CNY HNL</v>
       </c>
+      <c r="G14">
+        <v>3.49721</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -728,6 +737,9 @@
       <c r="F15" t="str">
         <v>EUR HNL</v>
       </c>
+      <c r="G15">
+        <v>25.7103</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -748,6 +760,9 @@
       <c r="F16" t="str">
         <v>GBP HNL</v>
       </c>
+      <c r="G16">
+        <v>29.0746</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -768,6 +783,9 @@
       <c r="F17" t="str">
         <v>JPY HNL</v>
       </c>
+      <c r="G17">
+        <v>0.17887</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -788,6 +806,9 @@
       <c r="F18" t="str">
         <v>MXN HNL</v>
       </c>
+      <c r="G18">
+        <v>1.3071</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -808,6 +829,9 @@
       <c r="F19" t="str">
         <v>HKD USD</v>
       </c>
+      <c r="G19">
+        <v>0.12743</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -827,6 +851,9 @@
       </c>
       <c r="F20" t="str">
         <v>HKD HNL</v>
+      </c>
+      <c r="G20">
+        <v>3.0783</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Subida de archivos de Testing
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -453,7 +453,7 @@
         <v>USD CRC</v>
       </c>
       <c r="C3" t="str">
-        <v>550.11</v>
+        <v>544.00</v>
       </c>
       <c r="D3" t="str">
         <v/>
@@ -465,7 +465,7 @@
         <v>EUR USD</v>
       </c>
       <c r="G3">
-        <v>1.07109</v>
+        <v>1.08786</v>
       </c>
     </row>
     <row r="4">
@@ -476,7 +476,7 @@
         <v>USD UYU</v>
       </c>
       <c r="C4">
-        <v>39.333</v>
+        <v>38.741</v>
       </c>
       <c r="D4" t="str">
         <v/>
@@ -488,7 +488,7 @@
         <v>EUR COP</v>
       </c>
       <c r="G4">
-        <v>NaN</v>
+        <v>4961.12</v>
       </c>
     </row>
     <row r="5">
@@ -511,7 +511,7 @@
         <v>CNY USD</v>
       </c>
       <c r="G5">
-        <v>0.14552</v>
+        <v>0.14535</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         <v>USD PEN</v>
       </c>
       <c r="C6">
-        <v>3.803</v>
+        <v>3.781</v>
       </c>
       <c r="D6" t="str">
         <v/>
@@ -534,7 +534,7 @@
         <v>JPY USD</v>
       </c>
       <c r="G6">
-        <v>0.00748</v>
+        <v>0.00752</v>
       </c>
     </row>
     <row r="7">
@@ -545,7 +545,7 @@
         <v>EUR PEN</v>
       </c>
       <c r="C7">
-        <v>4.367</v>
+        <v>4.385</v>
       </c>
       <c r="D7" t="str">
         <v/>
@@ -557,7 +557,7 @@
         <v>CNY COP</v>
       </c>
       <c r="G7">
-        <v>688.124</v>
+        <v>662.864</v>
       </c>
     </row>
     <row r="8">
@@ -568,7 +568,7 @@
         <v>USD CLP</v>
       </c>
       <c r="C8">
-        <v>797.19</v>
+        <v>821.49</v>
       </c>
       <c r="D8" t="str">
         <v/>
@@ -580,7 +580,7 @@
         <v>JPY COP</v>
       </c>
       <c r="G8">
-        <v>35.3935</v>
+        <v>34.2819</v>
       </c>
     </row>
     <row r="9">
@@ -591,7 +591,7 @@
         <v>EUR CLP</v>
       </c>
       <c r="C9">
-        <v>850.06</v>
+        <v>891.76</v>
       </c>
       <c r="D9" t="str">
         <v/>
@@ -603,7 +603,7 @@
         <v>BRL USD</v>
       </c>
       <c r="G9">
-        <v>0.19105</v>
+        <v>0.19738</v>
       </c>
     </row>
     <row r="10">
@@ -623,7 +623,7 @@
         <v>KRW USD</v>
       </c>
       <c r="G10">
-        <v>0.00077</v>
+        <v>0.00076</v>
       </c>
     </row>
     <row r="11">
@@ -633,9 +633,6 @@
       <c r="B11" t="str">
         <v>USD HNL</v>
       </c>
-      <c r="C11">
-        <v>NaN</v>
-      </c>
       <c r="D11" t="str">
         <v/>
       </c>
@@ -646,7 +643,7 @@
         <v>USD CLP</v>
       </c>
       <c r="G11">
-        <v>801.395</v>
+        <v>820.733</v>
       </c>
     </row>
     <row r="12">
@@ -669,7 +666,7 @@
         <v>EUR CLP</v>
       </c>
       <c r="G12">
-        <v>858.501</v>
+        <v>NaN</v>
       </c>
     </row>
     <row r="13">
@@ -691,9 +688,6 @@
       <c r="F13" t="str">
         <v>BRL HNL</v>
       </c>
-      <c r="G13">
-        <v>4.63299</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -714,9 +708,6 @@
       <c r="F14" t="str">
         <v>CNY HNL</v>
       </c>
-      <c r="G14">
-        <v>NaN</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -737,9 +728,6 @@
       <c r="F15" t="str">
         <v>EUR HNL</v>
       </c>
-      <c r="G15">
-        <v>25.9737</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -760,9 +748,6 @@
       <c r="F16" t="str">
         <v>GBP HNL</v>
       </c>
-      <c r="G16">
-        <v>29.4048</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -783,9 +768,6 @@
       <c r="F17" t="str">
         <v>JPY HNL</v>
       </c>
-      <c r="G17">
-        <v>0.1815</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -806,9 +788,6 @@
       <c r="F18" t="str">
         <v>MXN HNL</v>
       </c>
-      <c r="G18">
-        <v>1.29948</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -829,9 +808,6 @@
       <c r="F19" t="str">
         <v>HKD USD</v>
       </c>
-      <c r="G19">
-        <v>0.12748</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -851,9 +827,6 @@
       </c>
       <c r="F20" t="str">
         <v>HKD HNL</v>
-      </c>
-      <c r="G20">
-        <v>3.09125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>